<commit_message>
worked on console warnings
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testdata.xlsx
+++ b/src/test/resources/TestData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\AdvancedFrameworkOnline\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EAF72F-F373-4A68-8A81-2A0284C6CCBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C61521-6B74-433D-82F9-B325E274311F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4545" yWindow="2160" windowWidth="15300" windowHeight="7875" activeTab="1" xr2:uid="{1653A0DB-C2E4-5F45-84C3-178702117217}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>